<commit_message>
trained model with dataset 4, 5, 6
</commit_message>
<xml_diff>
--- a/Modelling/final report/Final_report_results.xlsx
+++ b/Modelling/final report/Final_report_results.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8796" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8796" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="SMO" sheetId="1" r:id="rId1"/>
-    <sheet name="BayesNet" sheetId="2" r:id="rId2"/>
-    <sheet name="J48" sheetId="3" r:id="rId3"/>
+    <sheet name="SMO_123" sheetId="1" r:id="rId1"/>
+    <sheet name="BayesNet_123" sheetId="2" r:id="rId2"/>
+    <sheet name="SMO_456" sheetId="4" r:id="rId3"/>
+    <sheet name="BayesNet_456" sheetId="5" r:id="rId4"/>
+    <sheet name="J48_456" sheetId="3" r:id="rId5"/>
+    <sheet name="Summary" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="354">
   <si>
     <t>=== Run information ===</t>
   </si>
@@ -355,18 +358,6 @@
     <t>=== Confusion Matrix ===</t>
   </si>
   <si>
-    <t xml:space="preserve">     a     b     c   &lt;-- classified as</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 13671    14    66 |     a = none</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    26   845     0 |     b = squeeze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    14     0   665 |     c = reach</t>
-  </si>
-  <si>
     <t>Scheme:weka.classifiers.bayes.BayesNet -D -Q weka.classifiers.bayes.net.search.local.K2 -- -P 1 -S BAYES -E weka.classifiers.bayes.net.estimate.SimpleEstimator -- -A 0.5</t>
   </si>
   <si>
@@ -490,20 +481,626 @@
     <t>Weighted Avg.    0.989     0.004      0.99      0.989     0.989      0.998</t>
   </si>
   <si>
-    <t xml:space="preserve"> 13591    54   106 |     a = none</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     1   868     2 |     b = squeeze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     5     0   674 |     c = reach</t>
+    <t>Instances:    23005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        -2.0267 * (normalized) meanLeft</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.269  * (normalized) meanRight</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       3.3717 * (normalized) varS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       1.0624 * (normalized) varS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       2.5693 * (normalized) varS3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       1.771  * (normalized) varS4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       3.2581 * (normalized) varS5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       1.6055 * (normalized) varS6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       1.5797 * (normalized) varS7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       1.2528 * (normalized) varS8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +      -0.2328 * (normalized) varS9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.7433 * (normalized) varS10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.7433 * (normalized) varS11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.7433 * (normalized) varS12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.7433 * (normalized) varS13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.7433 * (normalized) varS14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.7433 * (normalized) varS15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.7433 * (normalized) varS16</t>
+  </si>
+  <si>
+    <t>Number of kernel evaluations: 17988 (69.09% cached)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        -0.9676 * (normalized) meanLeft</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +      -6.2272 * (normalized) meanRight</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.0484 * (normalized) varS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +      -1.1031 * (normalized) varS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.0238 * (normalized) varS3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +      -1.2079 * (normalized) varS4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       1.1802 * (normalized) varS5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       1.6325 * (normalized) varS6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +      -4.7058 * (normalized) varS7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       3.662  * (normalized) varS8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.0007 * (normalized) varS9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       2.2354 * (normalized) varS10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       2.2354 * (normalized) varS11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       2.2354 * (normalized) varS12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       2.2354 * (normalized) varS13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       2.2354 * (normalized) varS14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       2.2354 * (normalized) varS15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       2.2354 * (normalized) varS16</t>
+  </si>
+  <si>
+    <t>Number of kernel evaluations: 59155 (66.984% cached)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0.4423 * (normalized) meanLeft</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +      -0.9885 * (normalized) meanRight</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +      -1.8738 * (normalized) varS1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +      -2.6968 * (normalized) varS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +      -5.0605 * (normalized) varS3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +      -3.8465 * (normalized) varS4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +      -0.8571 * (normalized) varS5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +      -1.2967 * (normalized) varS6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +      -2.0835 * (normalized) varS7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.6601 * (normalized) varS8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +      -0.0816 * (normalized) varS9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.9719 * (normalized) varS10</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.9719 * (normalized) varS11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.9719 * (normalized) varS12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.9719 * (normalized) varS13</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.9719 * (normalized) varS14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.9719 * (normalized) varS15</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +       0.9719 * (normalized) varS16</t>
+  </si>
+  <si>
+    <t>Number of kernel evaluations: 50523 (68.688% cached)</t>
+  </si>
+  <si>
+    <t>Time taken to build model: 0.36 seconds</t>
+  </si>
+  <si>
+    <t>Correctly Classified Instances       22807               99.1393 %</t>
+  </si>
+  <si>
+    <t>Incorrectly Classified Instances       198                0.8607 %</t>
+  </si>
+  <si>
+    <t>Kappa statistic                          0.9517</t>
+  </si>
+  <si>
+    <t>Mean absolute error                      0.2243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Root mean squared error                  0.276 </t>
+  </si>
+  <si>
+    <t>Relative absolute error                187.1808 %</t>
+  </si>
+  <si>
+    <t>Root relative squared error            112.7645 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Number of Instances            23005     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0.996     0.052      0.994     0.996     0.995      0.974    none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0.955     0.001      0.983     0.955     0.969      0.988    squeeze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0.94      0.003      0.95      0.94      0.945      0.969    reach</t>
+  </si>
+  <si>
+    <t>Weighted Avg.    0.991     0.047      0.991     0.991     0.991      0.974</t>
+  </si>
+  <si>
+    <t>Relation:     combined_1_2_3_r_4_5_6</t>
+  </si>
+  <si>
+    <t>Scheme:weka.classifiers.trees.J48 -C 0.25 -M 2</t>
+  </si>
+  <si>
+    <t>J48 pruned tree</t>
+  </si>
+  <si>
+    <t>------------------</t>
+  </si>
+  <si>
+    <t>varS10 &lt;= 288.34</t>
+  </si>
+  <si>
+    <t>|   meanLeft &lt;= 1005</t>
+  </si>
+  <si>
+    <t>|   |   varS1 &lt;= 784: none (6.0)</t>
+  </si>
+  <si>
+    <t>|   |   varS1 &gt; 784: squeeze (20.0/2.0)</t>
+  </si>
+  <si>
+    <t>|   meanLeft &gt; 1005</t>
+  </si>
+  <si>
+    <t>|   |   varS1 &lt;= 288.34</t>
+  </si>
+  <si>
+    <t>|   |   |   varS9 &lt;= 354.3: none (20578.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   varS9 &gt; 354.3</t>
+  </si>
+  <si>
+    <t>|   |   |   |   varS9 &lt;= 1528.66</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   varS2 &lt;= 0.94</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   varS3 &lt;= 0.96: none (6.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   varS3 &gt; 0.96: reach (3.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   varS2 &gt; 0.94: none (22.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   varS9 &gt; 1528.66: reach (2.0)</t>
+  </si>
+  <si>
+    <t>|   |   varS1 &gt; 288.34</t>
+  </si>
+  <si>
+    <t>|   |   |   varS9 &lt;= 87.84: none (14.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   varS9 &gt; 87.84</t>
+  </si>
+  <si>
+    <t>|   |   |   |   varS5 &lt;= 1703.84</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   varS10 &lt;= 15.86: none (2.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   varS10 &gt; 15.86: squeeze (6.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   varS5 &gt; 1703.84: none (4.0)</t>
+  </si>
+  <si>
+    <t>varS10 &gt; 288.34</t>
+  </si>
+  <si>
+    <t>|   varS4 &lt;= 9448.24</t>
+  </si>
+  <si>
+    <t>|   |   varS3 &lt;= 9600.1</t>
+  </si>
+  <si>
+    <t>|   |   |   varS7 &lt;= 1687.02</t>
+  </si>
+  <si>
+    <t>|   |   |   |   varS10 &lt;= 929.08</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   varS9 &lt;= 417.94: none (20.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   varS9 &gt; 417.94</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   meanLeft &lt;= 1021: none (6.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   meanLeft &gt; 1021</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   meanRight &lt;= 1002: reach (53.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   meanRight &gt; 1002</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   varS4 &lt;= 0.94: none (2.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   varS4 &gt; 0.94: reach (12.0/2.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   varS10 &gt; 929.08: reach (701.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   varS7 &gt; 1687.02</t>
+  </si>
+  <si>
+    <t>|   |   |   |   varS3 &lt;= 961</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   varS7 &lt;= 11108.26</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   varS8 &lt;= 1089</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   varS5 &lt;= 79.98</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   varS10 &lt;= 771.72: none (15.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   varS10 &gt; 771.72: reach (65.0/26.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   varS5 &gt; 79.98: none (52.0/2.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   varS8 &gt; 1089</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   varS5 &lt;= 3233.86: reach (67.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   varS5 &gt; 3233.86</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   varS5 &lt;= 6725.3: squeeze (3.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   |   |   varS5 &gt; 6725.3: reach (5.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   varS7 &gt; 11108.26: reach (101.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   varS3 &gt; 961</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   varS8 &lt;= 838.72: none (3.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   varS8 &gt; 838.72</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   meanLeft &lt;= 994: reach (380.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   |   meanLeft &gt; 994: squeeze (21.0)</t>
+  </si>
+  <si>
+    <t>|   |   varS3 &gt; 9600.1: squeeze (132.0)</t>
+  </si>
+  <si>
+    <t>|   varS4 &gt; 9448.24</t>
+  </si>
+  <si>
+    <t>|   |   varS1 &lt;= 1087.7</t>
+  </si>
+  <si>
+    <t>|   |   |   varS10 &lt;= 574.12</t>
+  </si>
+  <si>
+    <t>|   |   |   |   varS10 &lt;= 501.32: none (9.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   varS10 &gt; 501.32</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   varS2 &lt;= 27050.64: squeeze (2.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   |   |   varS2 &gt; 27050.64: none (3.0)</t>
+  </si>
+  <si>
+    <t>|   |   |   varS10 &gt; 574.12: squeeze (14.0/1.0)</t>
+  </si>
+  <si>
+    <t>|   |   varS1 &gt; 1087.7: squeeze (676.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Leaves  : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size of the tree : </t>
+  </si>
+  <si>
+    <t>Time taken to build model: 1.05 seconds</t>
+  </si>
+  <si>
+    <t>Correctly Classified Instances       22925               99.6522 %</t>
+  </si>
+  <si>
+    <t>Incorrectly Classified Instances        80                0.3478 %</t>
+  </si>
+  <si>
+    <t>Kappa statistic                          0.9807</t>
+  </si>
+  <si>
+    <t>Mean absolute error                      0.0028</t>
+  </si>
+  <si>
+    <t>Root mean squared error                  0.0454</t>
+  </si>
+  <si>
+    <t>Relative absolute error                  2.3636 %</t>
+  </si>
+  <si>
+    <t>Root relative squared error             18.5318 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0.998     0.011      0.999     0.998     0.998      0.996    none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0.982     0.001      0.985     0.982     0.983      0.992    squeeze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0.985     0.002      0.97      0.985     0.977      0.994    reach</t>
+  </si>
+  <si>
+    <t>Weighted Avg.    0.997     0.01       0.997     0.997     0.997      0.995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meanLeft(12): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">meanRight(13): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS1(18): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS2(19): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS3(15): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS4(9): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS5(13): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS6(13): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS7(22): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS8(15): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS9(25): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS10(22): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS11(22): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS12(22): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS13(22): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS14(22): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS15(22): class </t>
+  </si>
+  <si>
+    <t xml:space="preserve">varS16(22): class </t>
+  </si>
+  <si>
+    <t>LogScore Bayes: -249631.628885302</t>
+  </si>
+  <si>
+    <t>LogScore BDeu: -253580.75062349808</t>
+  </si>
+  <si>
+    <t>LogScore MDL: -254199.3972173271</t>
+  </si>
+  <si>
+    <t>LogScore ENTROPY: -249519.14165936035</t>
+  </si>
+  <si>
+    <t>LogScore AIC: -250451.14165936035</t>
+  </si>
+  <si>
+    <t>Time taken to build model: 0.51 seconds</t>
+  </si>
+  <si>
+    <t>Correctly Classified Instances       22729               98.8003 %</t>
+  </si>
+  <si>
+    <t>Incorrectly Classified Instances       276                1.1997 %</t>
+  </si>
+  <si>
+    <t>Kappa statistic                          0.9357</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean absolute error                      0.008 </t>
+  </si>
+  <si>
+    <t>Root mean squared error                  0.0876</t>
+  </si>
+  <si>
+    <t>Relative absolute error                  6.7029 %</t>
+  </si>
+  <si>
+    <t>Root relative squared error             35.7958 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0.991     0.004      1         0.991     0.995      0.999    none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0.975     0.004      0.899     0.975     0.936      0.999    squeeze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 0.956     0.008      0.883     0.956     0.918      0.998    reach</t>
+  </si>
+  <si>
+    <t>Weighted Avg.    0.988     0.004      0.989     0.988     0.988      0.999</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>a = none</t>
+  </si>
+  <si>
+    <t>b = squeeze</t>
+  </si>
+  <si>
+    <t>c = reach</t>
+  </si>
+  <si>
+    <t>classified as</t>
+  </si>
+  <si>
+    <t>initial dataset</t>
+  </si>
+  <si>
+    <t>expanded dataset</t>
+  </si>
+  <si>
+    <t>BayesNet</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Squeeze</t>
+  </si>
+  <si>
+    <t>Reach</t>
+  </si>
+  <si>
+    <t>Model training crossvalidation</t>
+  </si>
+  <si>
+    <t>Model for evaluation</t>
+  </si>
+  <si>
+    <t>J48</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,16 +1108,79 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -528,15 +1188,328 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="3" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="4" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="5" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="6" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="12" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="11" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="12" xfId="5" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="16" xfId="7" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="17" xfId="7" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="19" xfId="7" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="8">
+    <cellStyle name="40% - Accent2" xfId="3" builtinId="35"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="40% - Accent6" xfId="7" builtinId="51"/>
+    <cellStyle name="Accent2" xfId="2" builtinId="33"/>
+    <cellStyle name="Accent5" xfId="4" builtinId="45"/>
+    <cellStyle name="Accent6" xfId="6" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -814,10 +1787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A148"/>
+  <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="F146" sqref="F146:F148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1402,24 +2375,72 @@
         <v>108</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A145" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A146" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A147" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A148" t="s">
-        <v>112</v>
+    <row r="145" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B145" t="s">
+        <v>338</v>
+      </c>
+      <c r="C145" t="s">
+        <v>339</v>
+      </c>
+      <c r="D145" t="s">
+        <v>340</v>
+      </c>
+      <c r="E145" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="146" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B146">
+        <v>13671</v>
+      </c>
+      <c r="C146">
+        <v>14</v>
+      </c>
+      <c r="D146">
+        <v>66</v>
+      </c>
+      <c r="E146" t="s">
+        <v>341</v>
+      </c>
+      <c r="F146" s="1">
+        <f>B146/SUM(B146:D146)</f>
+        <v>0.99418224129154242</v>
+      </c>
+    </row>
+    <row r="147" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B147">
+        <v>26</v>
+      </c>
+      <c r="C147">
+        <v>845</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147" t="s">
+        <v>342</v>
+      </c>
+      <c r="F147" s="1">
+        <f>C147/SUM(B147:D147)</f>
+        <v>0.97014925373134331</v>
+      </c>
+    </row>
+    <row r="148" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B148">
+        <v>14</v>
+      </c>
+      <c r="C148">
+        <v>0</v>
+      </c>
+      <c r="D148">
+        <v>665</v>
+      </c>
+      <c r="E148" t="s">
+        <v>343</v>
+      </c>
+      <c r="F148" s="1">
+        <f>D148/SUM(B148:D148)</f>
+        <v>0.97938144329896903</v>
       </c>
     </row>
   </sheetData>
@@ -1429,10 +2450,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A87"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F85" sqref="F85:F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1444,7 +2465,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -1569,147 +2590,147 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -1724,37 +2745,37 @@
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.55000000000000004">
@@ -1774,47 +2795,95 @@
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" t="s">
-        <v>156</v>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B84" t="s">
+        <v>338</v>
+      </c>
+      <c r="C84" t="s">
+        <v>339</v>
+      </c>
+      <c r="D84" t="s">
+        <v>340</v>
+      </c>
+      <c r="E84" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B85">
+        <v>13591</v>
+      </c>
+      <c r="C85">
+        <v>54</v>
+      </c>
+      <c r="D85">
+        <v>106</v>
+      </c>
+      <c r="E85" t="s">
+        <v>341</v>
+      </c>
+      <c r="F85" s="1">
+        <f>B85/SUM(B85:D85)</f>
+        <v>0.98836448258308485</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>868</v>
+      </c>
+      <c r="D86">
+        <v>2</v>
+      </c>
+      <c r="E86" t="s">
+        <v>342</v>
+      </c>
+      <c r="F86" s="1">
+        <f>C86/SUM(B86:D86)</f>
+        <v>0.99655568312284726</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B87">
+        <v>5</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>674</v>
+      </c>
+      <c r="E87" t="s">
+        <v>343</v>
+      </c>
+      <c r="F87" s="1">
+        <f>D87/SUM(B87:D87)</f>
+        <v>0.99263622974963184</v>
       </c>
     </row>
   </sheetData>
@@ -1824,12 +2893,1896 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="F146" sqref="F146:F148"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>0.22739999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87">
+        <v>6.0515999999999996</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115">
+        <v>1.4280999999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="145" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B145" t="s">
+        <v>338</v>
+      </c>
+      <c r="C145" t="s">
+        <v>339</v>
+      </c>
+      <c r="D145" t="s">
+        <v>340</v>
+      </c>
+      <c r="E145" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="146" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B146">
+        <v>20696</v>
+      </c>
+      <c r="C146">
+        <v>14</v>
+      </c>
+      <c r="D146">
+        <v>63</v>
+      </c>
+      <c r="E146" t="s">
+        <v>341</v>
+      </c>
+      <c r="F146" s="1">
+        <f>B146/SUM(B146:D146)</f>
+        <v>0.99629326529629803</v>
+      </c>
+    </row>
+    <row r="147" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B147">
+        <v>34</v>
+      </c>
+      <c r="C147">
+        <v>832</v>
+      </c>
+      <c r="D147">
+        <v>5</v>
+      </c>
+      <c r="E147" t="s">
+        <v>342</v>
+      </c>
+      <c r="F147" s="1">
+        <f>C147/SUM(B147:D147)</f>
+        <v>0.95522388059701491</v>
+      </c>
+    </row>
+    <row r="148" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B148">
+        <v>82</v>
+      </c>
+      <c r="C148">
+        <v>0</v>
+      </c>
+      <c r="D148">
+        <v>1279</v>
+      </c>
+      <c r="E148" t="s">
+        <v>343</v>
+      </c>
+      <c r="F148" s="1">
+        <f>D148/SUM(B148:D148)</f>
+        <v>0.93975018368846441</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F87"/>
+  <sheetViews>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F85" sqref="F85:F87"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="5" max="5" width="9.83984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B84" t="s">
+        <v>338</v>
+      </c>
+      <c r="C84" t="s">
+        <v>339</v>
+      </c>
+      <c r="D84" t="s">
+        <v>340</v>
+      </c>
+      <c r="E84" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B85">
+        <v>20579</v>
+      </c>
+      <c r="C85">
+        <v>42</v>
+      </c>
+      <c r="D85">
+        <v>152</v>
+      </c>
+      <c r="E85" t="s">
+        <v>341</v>
+      </c>
+      <c r="F85" s="1">
+        <f>B85/SUM(B85:D85)</f>
+        <v>0.99066095412314059</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86">
+        <v>849</v>
+      </c>
+      <c r="D86">
+        <v>21</v>
+      </c>
+      <c r="E86" t="s">
+        <v>342</v>
+      </c>
+      <c r="F86" s="1">
+        <f>C86/SUM(B86:D86)</f>
+        <v>0.97474167623421359</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B87">
+        <v>7</v>
+      </c>
+      <c r="C87">
+        <v>53</v>
+      </c>
+      <c r="D87">
+        <v>1301</v>
+      </c>
+      <c r="E87" t="s">
+        <v>343</v>
+      </c>
+      <c r="F87" s="1">
+        <f>D87/SUM(B87:D87)</f>
+        <v>0.95591476855253488</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F130"/>
+  <sheetViews>
+    <sheetView topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="F128" sqref="F128:F130"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="5" max="5" width="9.83984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" t="s">
+        <v>289</v>
+      </c>
+      <c r="B98">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" t="s">
+        <v>290</v>
+      </c>
+      <c r="B100">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B127" t="s">
+        <v>338</v>
+      </c>
+      <c r="C127" t="s">
+        <v>339</v>
+      </c>
+      <c r="D127" t="s">
+        <v>340</v>
+      </c>
+      <c r="E127" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B128">
+        <v>20729</v>
+      </c>
+      <c r="C128">
+        <v>9</v>
+      </c>
+      <c r="D128">
+        <v>35</v>
+      </c>
+      <c r="E128" t="s">
+        <v>341</v>
+      </c>
+      <c r="F128" s="1">
+        <f>B128/SUM(B128:D128)</f>
+        <v>0.99788186588359895</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B129">
+        <v>9</v>
+      </c>
+      <c r="C129">
+        <v>855</v>
+      </c>
+      <c r="D129">
+        <v>7</v>
+      </c>
+      <c r="E129" t="s">
+        <v>342</v>
+      </c>
+      <c r="F129" s="1">
+        <f>C129/SUM(B129:D129)</f>
+        <v>0.98163030998851897</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B130">
+        <v>16</v>
+      </c>
+      <c r="C130">
+        <v>4</v>
+      </c>
+      <c r="D130">
+        <v>1341</v>
+      </c>
+      <c r="E130" t="s">
+        <v>343</v>
+      </c>
+      <c r="F130" s="1">
+        <f>D130/SUM(B130:D130)</f>
+        <v>0.98530492285084492</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="9" max="9" width="17.3125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="C2" t="s">
+        <v>351</v>
+      </c>
+      <c r="I2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="I3" s="30" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B4" s="14"/>
+      <c r="C4" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="28" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="19" t="s">
+        <v>348</v>
+      </c>
+      <c r="C5" s="20">
+        <v>0.99418224129154242</v>
+      </c>
+      <c r="D5" s="21">
+        <v>0.98836448258308485</v>
+      </c>
+      <c r="E5" s="22">
+        <v>0.99629326529629803</v>
+      </c>
+      <c r="F5" s="23">
+        <v>0.99066095412314059</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="19" t="s">
+        <v>348</v>
+      </c>
+      <c r="I5" s="29">
+        <v>0.99788186588359895</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.97014925373134331</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.99655568312284726</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.95522388059701491</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0.97474167623421359</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="24" t="s">
+        <v>349</v>
+      </c>
+      <c r="I6" s="26">
+        <v>0.98163030998851897</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="B7" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.97938144329896903</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.99263622974963184</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0.93975018368846441</v>
+      </c>
+      <c r="F7" s="13">
+        <v>0.95591476855253488</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="I7" s="27">
+        <v>0.98530492285084492</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>